<commit_message>
Filled out the dialogue table.
</commit_message>
<xml_diff>
--- a/src/main/Resources/spreadsheets/dialogue.xlsx
+++ b/src/main/Resources/spreadsheets/dialogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/devel/ShootingStars/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F9D8AA-75B5-214C-9FE5-02379A95291A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD72FE0-3162-0848-8F73-482F72AB859F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2120" windowWidth="28040" windowHeight="17440" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
+    <workbookView xWindow="16720" yWindow="860" windowWidth="17480" windowHeight="20540" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
   <sheets>
     <sheet name="dialogue" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>DIALOGUE</t>
   </si>
@@ -44,25 +44,172 @@
     <t>english</t>
   </si>
   <si>
-    <t>language display name</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
     <t>czech</t>
   </si>
   <si>
-    <t>Czech</t>
-  </si>
-  <si>
-    <t>app name</t>
-  </si>
-  <si>
     <t>Shooting Stars</t>
   </si>
   <si>
     <t>Padající Hvězdy</t>
+  </si>
+  <si>
+    <t>korean</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>Čeština</t>
+  </si>
+  <si>
+    <t>headingFont</t>
+  </si>
+  <si>
+    <t>textFont</t>
+  </si>
+  <si>
+    <t>languageDisplayName</t>
+  </si>
+  <si>
+    <t>appName</t>
+  </si>
+  <si>
+    <t>menuSubText</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>topscore</t>
+  </si>
+  <si>
+    <t>timeLeft</t>
+  </si>
+  <si>
+    <t>gameOver</t>
+  </si>
+  <si>
+    <t>gameOverSubtext</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>Press any key to continue</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Top score</t>
+  </si>
+  <si>
+    <t>Time left</t>
+  </si>
+  <si>
+    <t>GAME OVER</t>
+  </si>
+  <si>
+    <t>Press "R" to restart</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Stiskněte libovolnou klávesu pro pokračování</t>
+  </si>
+  <si>
+    <t>Skóre</t>
+  </si>
+  <si>
+    <t>Nejlepší skóre</t>
+  </si>
+  <si>
+    <t>Zbývající čas</t>
+  </si>
+  <si>
+    <t>KONEC HRY</t>
+  </si>
+  <si>
+    <t>Stiskněte "R" pro restart</t>
+  </si>
+  <si>
+    <t>Pozastaveno</t>
+  </si>
+  <si>
+    <t>별을 쏘다</t>
+  </si>
+  <si>
+    <t>한국인</t>
+  </si>
+  <si>
+    <t>아무 키나 누르세요 계속하려면</t>
+  </si>
+  <si>
+    <t>점수</t>
+  </si>
+  <si>
+    <t>최고 점수</t>
+  </si>
+  <si>
+    <t>남은 시간</t>
+  </si>
+  <si>
+    <t>게임 오버</t>
+  </si>
+  <si>
+    <t>다시 시작하려면 "R"을 누르세요</t>
+  </si>
+  <si>
+    <t>일시 정지</t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>続行するには任意のキーを押してください</t>
+  </si>
+  <si>
+    <t>流れ星撃ち</t>
+  </si>
+  <si>
+    <t>スコア</t>
+  </si>
+  <si>
+    <t>トプスコア</t>
+  </si>
+  <si>
+    <t>残り時間</t>
+  </si>
+  <si>
+    <t>ゲームオーバー</t>
+  </si>
+  <si>
+    <t>再起動するには "R" を押してください</t>
+  </si>
+  <si>
+    <t>一時停止</t>
+  </si>
+  <si>
+    <t>heading_EN.tff</t>
+  </si>
+  <si>
+    <t>text_EN.tff</t>
+  </si>
+  <si>
+    <t>text_CZ.tff</t>
+  </si>
+  <si>
+    <t>heading_KOR.tff</t>
+  </si>
+  <si>
+    <t>heading_JAP.otf</t>
+  </si>
+  <si>
+    <t>text_JAP.otf</t>
   </si>
 </sst>
 </file>
@@ -482,21 +629,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2AB3D20-1825-A34C-8076-B43BF1C24F7C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="19.33203125" style="1"/>
+    <col min="2" max="2" width="51.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="73.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="19.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -504,29 +654,200 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working language spreadsheet integration.
</commit_message>
<xml_diff>
--- a/src/main/Resources/spreadsheets/dialogue.xlsx
+++ b/src/main/Resources/spreadsheets/dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/devel/ShootingStars/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD72FE0-3162-0848-8F73-482F72AB859F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B721A784-57AD-C64A-BEC6-1E929D1FFBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16720" yWindow="860" windowWidth="17480" windowHeight="20540" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>DIALOGUE</t>
   </si>
@@ -50,9 +50,6 @@
     <t>czech</t>
   </si>
   <si>
-    <t>Shooting Stars</t>
-  </si>
-  <si>
     <t>Padající Hvězdy</t>
   </si>
   <si>
@@ -194,22 +191,28 @@
     <t>一時停止</t>
   </si>
   <si>
-    <t>heading_EN.tff</t>
-  </si>
-  <si>
-    <t>text_EN.tff</t>
-  </si>
-  <si>
-    <t>text_CZ.tff</t>
-  </si>
-  <si>
-    <t>heading_KOR.tff</t>
-  </si>
-  <si>
     <t>heading_JAP.otf</t>
   </si>
   <si>
     <t>text_JAP.otf</t>
+  </si>
+  <si>
+    <t>heading_EN.ttf</t>
+  </si>
+  <si>
+    <t>text_CZ.ttf</t>
+  </si>
+  <si>
+    <t>text_EN.ttf</t>
+  </si>
+  <si>
+    <t>heading_KOR.ttf</t>
+  </si>
+  <si>
+    <t>Shooting Stars :3</t>
+  </si>
+  <si>
+    <t>defaultFont</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -657,197 +660,197 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code formating, removed debug methods & messages.
</commit_message>
<xml_diff>
--- a/src/main/Resources/spreadsheets/dialogue.xlsx
+++ b/src/main/Resources/spreadsheets/dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/devel/ShootingStars/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B721A784-57AD-C64A-BEC6-1E929D1FFBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74BF623-1B8A-4445-A077-4CEFFD81B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16720" yWindow="860" windowWidth="17480" windowHeight="20540" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
@@ -50,6 +50,9 @@
     <t>czech</t>
   </si>
   <si>
+    <t>Shooting Stars</t>
+  </si>
+  <si>
     <t>Padající Hvězdy</t>
   </si>
   <si>
@@ -207,9 +210,6 @@
   </si>
   <si>
     <t>heading_KOR.ttf</t>
-  </si>
-  <si>
-    <t>Shooting Stars :3</t>
   </si>
   <si>
     <t>defaultFont</t>
@@ -635,8 +635,8 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -660,197 +660,197 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited the dialogue, and the readme to reflect the keybind changes.
</commit_message>
<xml_diff>
--- a/src/main/Resources/spreadsheets/dialogue.xlsx
+++ b/src/main/Resources/spreadsheets/dialogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/devel/ShootingStars/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74BF623-1B8A-4445-A077-4CEFFD81B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A0962B-A061-0945-9200-9541F1FD14DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16720" yWindow="860" windowWidth="17480" windowHeight="20540" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
   <sheets>
     <sheet name="dialogue" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>pause</t>
   </si>
   <si>
-    <t>Press any key to continue</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Pause</t>
   </si>
   <si>
-    <t>Stiskněte libovolnou klávesu pro pokračování</t>
-  </si>
-  <si>
     <t>Skóre</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>한국인</t>
   </si>
   <si>
-    <t>아무 키나 누르세요 계속하려면</t>
-  </si>
-  <si>
     <t>점수</t>
   </si>
   <si>
@@ -161,18 +152,12 @@
     <t>게임 오버</t>
   </si>
   <si>
-    <t>다시 시작하려면 "R"을 누르세요</t>
-  </si>
-  <si>
     <t>일시 정지</t>
   </si>
   <si>
     <t>日本語</t>
   </si>
   <si>
-    <t>続行するには任意のキーを押してください</t>
-  </si>
-  <si>
     <t>流れ星撃ち</t>
   </si>
   <si>
@@ -188,9 +173,6 @@
     <t>ゲームオーバー</t>
   </si>
   <si>
-    <t>再起動するには "R" を押してください</t>
-  </si>
-  <si>
     <t>一時停止</t>
   </si>
   <si>
@@ -213,6 +195,24 @@
   </si>
   <si>
     <t>defaultFont</t>
+  </si>
+  <si>
+    <t>再起動するには 「R」 を押してください</t>
+  </si>
+  <si>
+    <t>다시 시작하려면 ‘R’ 을 누르세요</t>
+  </si>
+  <si>
+    <t>Press the "S" key to start</t>
+  </si>
+  <si>
+    <t>「S」キーを押してスタートしてください</t>
+  </si>
+  <si>
+    <t>‘R’ 키를 눌러 시작하세요</t>
+  </si>
+  <si>
+    <t>Stiskněte klávesu “S” pro spuštění</t>
   </si>
 </sst>
 </file>
@@ -284,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,6 +296,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,9 +637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2AB3D20-1825-A34C-8076-B43BF1C24F7C}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection pane="topRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -671,16 +674,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -688,16 +691,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -711,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -728,10 +731,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -739,16 +742,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -756,16 +759,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -773,16 +776,16 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -790,16 +793,16 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -807,16 +810,16 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -824,16 +827,16 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -841,19 +844,20 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>